<commit_message>
voltage commutation possible with ecu v1.0
- voltage commutation work fine
- adc is configurable with 2 option either regular conversion on 7-16 channels ot only 4 channels injection
- conversion of currents and dc link possible
- update suitable with the assembled setup (ecu v1.0)
</commit_message>
<xml_diff>
--- a/DOCS/config.xlsx
+++ b/DOCS/config.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive - Continental AG\Work\_Simulations\STM\BLDC_HALL-master\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B07C0791-48A6-4176-996E-6024EF63A9C7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC1FC5CD-2B05-45C4-A97D-7E4C853948B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{D3E645C1-CD67-4302-919E-24FF7288B4B0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{D3E645C1-CD67-4302-919E-24FF7288B4B0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ADC" sheetId="1" r:id="rId1"/>
+    <sheet name="PWM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ADC channel sampling time</t>
   </si>
@@ -52,14 +53,43 @@
   </si>
   <si>
     <t>Total Conversion time(ns)</t>
+  </si>
+  <si>
+    <t>PWM period</t>
+  </si>
+  <si>
+    <t>Prescaler</t>
+  </si>
+  <si>
+    <t>APB2 Freq</t>
+  </si>
+  <si>
+    <t>TIM Freq</t>
+  </si>
+  <si>
+    <t>ARR</t>
+  </si>
+  <si>
+    <t>PWM Freq</t>
+  </si>
+  <si>
+    <t>Tcnt</t>
+  </si>
+  <si>
+    <t>ADC Sampling duration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="6">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;lei&quot;;[Red]\-#,##0.00\ &quot;lei&quot;"/>
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
+    <numFmt numFmtId="173" formatCode="0.00000"/>
+    <numFmt numFmtId="177" formatCode="0.000000000"/>
+    <numFmt numFmtId="178" formatCode="0.00000000000"/>
+    <numFmt numFmtId="179" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -91,12 +121,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,14 +449,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B154BFE-5834-48FF-9923-FDB5DF07089E}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -437,6 +475,10 @@
       <c r="B2">
         <v>84000000</v>
       </c>
+      <c r="C2" s="5">
+        <f>1/B2</f>
+        <v>1.1904761904761905E-8</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -450,9 +492,17 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <f>B2/B3</f>
         <v>21000000</v>
+      </c>
+      <c r="C4" s="7">
+        <f>1/B4</f>
+        <v>4.761904761904762E-8</v>
+      </c>
+      <c r="D4" s="5">
+        <f>C2*4</f>
+        <v>4.761904761904762E-8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -468,7 +518,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -477,7 +527,7 @@
       </c>
       <c r="B8" s="1">
         <f>(B6+B7)*(1/B4)</f>
-        <v>7.1428571428571431E-7</v>
+        <v>4.5714285714285719E-6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -485,20 +535,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="6">
         <f>B8*B9</f>
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="D11">
-        <f>702.85+222.85+45.71</f>
-        <v>971.41000000000008</v>
+        <v>1.8285714285714288E-5</v>
       </c>
     </row>
   </sheetData>
@@ -508,4 +554,103 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629A1D58-3D10-4E20-A8A6-9B6E561AAFA9}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>84000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <f>B2/(B3+1)</f>
+        <v>84000000</v>
+      </c>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="7">
+        <f>(1/B4)*1000000</f>
+        <v>1.1904761904761906E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <f>1290*B5</f>
+        <v>15.357142857142858</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>4199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f>B4/(B9+1)</f>
+        <v>20000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>